<commit_message>
Updtade P18 for STM32F407 and FRDM boards
Signed-off-by: Jose Leitao <jose.p.leitao@gmail.com>
</commit_message>
<xml_diff>
--- a/STM32F407/pinos.xlsx
+++ b/STM32F407/pinos.xlsx
@@ -1589,8 +1589,8 @@
   <dimension ref="A1:S145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>